<commit_message>
Chạy kết quả thực nghiệm với thời gian trong threshold 40 và 123
</commit_message>
<xml_diff>
--- a/BaoCao.xlsx
+++ b/BaoCao.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Threshold=123" sheetId="1" r:id="rId1"/>
+    <sheet name="Threshold=40" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>Lần 1</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Thực nghiệm thực hiện với threshold = 123.0</t>
+  </si>
+  <si>
+    <t>Thời gian thực hiện (dvt: giây)</t>
+  </si>
+  <si>
+    <t>Thực nghiệm thực hiện với threshold = 40</t>
   </si>
 </sst>
 </file>
@@ -183,10 +189,10 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -491,35 +497,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -659,20 +665,40 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4">
+        <v>24</v>
+      </c>
+      <c r="I8" s="4">
+        <v>24</v>
+      </c>
+      <c r="J8" s="4">
+        <v>24</v>
+      </c>
+      <c r="K8" s="4">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -710,16 +736,16 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -863,16 +889,36 @@
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="B17" s="4">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4">
+        <v>23</v>
+      </c>
+      <c r="G17" s="4">
+        <v>23</v>
+      </c>
+      <c r="H17" s="4">
+        <v>23</v>
+      </c>
+      <c r="I17" s="4">
+        <v>24</v>
+      </c>
+      <c r="J17" s="4">
+        <v>24</v>
+      </c>
+      <c r="K17" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -935,12 +981,505 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <v>200</v>
+      </c>
+      <c r="C5" s="4">
+        <v>200</v>
+      </c>
+      <c r="D5" s="4">
+        <v>200</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" s="4">
+        <v>200</v>
+      </c>
+      <c r="G5" s="4">
+        <v>200</v>
+      </c>
+      <c r="H5" s="4">
+        <v>200</v>
+      </c>
+      <c r="I5" s="4">
+        <v>200</v>
+      </c>
+      <c r="J5" s="4">
+        <v>200</v>
+      </c>
+      <c r="K5" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4">
+        <v>200</v>
+      </c>
+      <c r="C6" s="4">
+        <v>200</v>
+      </c>
+      <c r="D6" s="4">
+        <v>200</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" s="4">
+        <v>200</v>
+      </c>
+      <c r="G6" s="4">
+        <v>200</v>
+      </c>
+      <c r="H6" s="4">
+        <v>200</v>
+      </c>
+      <c r="I6" s="4">
+        <v>200</v>
+      </c>
+      <c r="J6" s="4">
+        <v>200</v>
+      </c>
+      <c r="K6" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4">
+        <v>92</v>
+      </c>
+      <c r="D7" s="4">
+        <v>112</v>
+      </c>
+      <c r="E7" s="4">
+        <v>109</v>
+      </c>
+      <c r="F7" s="4">
+        <v>90</v>
+      </c>
+      <c r="G7" s="4">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4">
+        <v>99</v>
+      </c>
+      <c r="I7" s="4">
+        <v>106</v>
+      </c>
+      <c r="J7" s="4">
+        <v>109</v>
+      </c>
+      <c r="K7" s="4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4">
+        <v>23</v>
+      </c>
+      <c r="H8" s="4">
+        <v>23</v>
+      </c>
+      <c r="I8" s="4">
+        <v>23</v>
+      </c>
+      <c r="J8" s="4">
+        <v>23</v>
+      </c>
+      <c r="K8" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B7/B6</f>
+        <v>0.38</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" ref="C9:J9" si="0">C7/C6</f>
+        <v>0.46</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.495</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ref="C9:K9" si="1">ROUND((K7/K6),2)</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4">
+        <v>80</v>
+      </c>
+      <c r="E14" s="4">
+        <v>100</v>
+      </c>
+      <c r="F14" s="4">
+        <v>120</v>
+      </c>
+      <c r="G14" s="4">
+        <v>140</v>
+      </c>
+      <c r="H14" s="4">
+        <v>160</v>
+      </c>
+      <c r="I14" s="4">
+        <v>180</v>
+      </c>
+      <c r="J14" s="4">
+        <v>200</v>
+      </c>
+      <c r="K14" s="4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>360</v>
+      </c>
+      <c r="C15" s="4">
+        <v>340</v>
+      </c>
+      <c r="D15" s="4">
+        <v>320</v>
+      </c>
+      <c r="E15" s="4">
+        <v>300</v>
+      </c>
+      <c r="F15" s="4">
+        <v>280</v>
+      </c>
+      <c r="G15" s="4">
+        <v>260</v>
+      </c>
+      <c r="H15" s="4">
+        <v>240</v>
+      </c>
+      <c r="I15" s="4">
+        <v>220</v>
+      </c>
+      <c r="J15" s="4">
+        <v>200</v>
+      </c>
+      <c r="K15" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>67</v>
+      </c>
+      <c r="C16" s="4">
+        <v>82</v>
+      </c>
+      <c r="D16" s="4">
+        <v>90</v>
+      </c>
+      <c r="E16" s="4">
+        <v>111</v>
+      </c>
+      <c r="F16" s="4">
+        <v>121</v>
+      </c>
+      <c r="G16" s="4">
+        <v>113</v>
+      </c>
+      <c r="H16" s="4">
+        <v>115</v>
+      </c>
+      <c r="I16" s="4">
+        <v>94</v>
+      </c>
+      <c r="J16" s="4">
+        <v>90</v>
+      </c>
+      <c r="K16" s="4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4">
+        <v>23</v>
+      </c>
+      <c r="F17" s="4">
+        <v>22</v>
+      </c>
+      <c r="G17" s="4">
+        <v>23</v>
+      </c>
+      <c r="H17" s="4">
+        <v>23</v>
+      </c>
+      <c r="I17" s="4">
+        <v>23</v>
+      </c>
+      <c r="J17" s="4">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B16/B15</f>
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" ref="C18:K18" si="2">C16/C15</f>
+        <v>0.2411764705882353</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.28125</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.37</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.43214285714285716</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.43461538461538463</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.42727272727272725</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="2"/>
+        <v>0.51666666666666672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A12:H12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Uơdate file thưc nghiem
</commit_message>
<xml_diff>
--- a/BaoCao.xlsx
+++ b/BaoCao.xlsx
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -165,11 +173,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -194,6 +230,16 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,20 +543,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -595,7 +650,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -630,7 +685,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -665,7 +720,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -700,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -780,7 +835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -815,7 +870,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -850,7 +905,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -885,7 +940,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -920,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -955,24 +1010,24 @@
         <v>0.89439999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -983,20 +1038,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -1046,7 +1104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1139,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1116,7 +1174,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1209,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1186,7 +1244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1227,7 +1285,7 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" ref="C9:K9" si="1">ROUND((K7/K6),2)</f>
+        <f t="shared" ref="K9" si="1">ROUND((K7/K6),2)</f>
         <v>0.52</v>
       </c>
     </row>
@@ -1276,7 +1334,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1311,7 +1369,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1404,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1381,7 +1439,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1416,7 +1474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>